<commit_message>
Update the invalide test data for script: TD_NGQ_CPQ_EncoreRetirement_US9408_AddTSCustomServicesToEachConfigurationSolution_08
</commit_message>
<xml_diff>
--- a/data/TD_NGQ_CPQ_EncoreRetirement_US9408_AddTSCustomServicesToEachConfigurationSolution_08.xlsx
+++ b/data/TD_NGQ_CPQ_EncoreRetirement_US9408_AddTSCustomServicesToEachConfigurationSolution_08.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ngq-demo-develop\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="816" windowWidth="23040" windowHeight="8988"/>
+    <workbookView xWindow="0" yWindow="810" windowWidth="23040" windowHeight="8985"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,7 +45,7 @@
     <t>ProductNumberB</t>
   </si>
   <si>
-    <t>H1K92A3</t>
+    <t>AJ715AR</t>
   </si>
 </sst>
 </file>
@@ -360,7 +355,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -371,12 +366,12 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>